<commit_message>
data and color update
</commit_message>
<xml_diff>
--- a/R/teamcolors.xlsx
+++ b/R/teamcolors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roger\Documents\GitHub\All-Star-Predictions\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49351E5A-6D07-4170-BDB6-5A89EE9A7966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36EABAE-00E2-4D5C-ADF1-A50DC4959047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{33173667-A529-4C81-BB71-477202676060}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>Team</t>
   </si>
@@ -271,9 +271,6 @@
     <t>WAS</t>
   </si>
   <si>
-    <t>#FDB927</t>
-  </si>
-  <si>
     <t>#00788C</t>
   </si>
   <si>
@@ -299,6 +296,15 @@
   </si>
   <si>
     <t>#78BE20</t>
+  </si>
+  <si>
+    <t>#F1AA11</t>
+  </si>
+  <si>
+    <t>#753BBD</t>
+  </si>
+  <si>
+    <t>#BA0C2F</t>
   </si>
 </sst>
 </file>
@@ -653,7 +659,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +719,7 @@
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +763,7 @@
         <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,7 +796,7 @@
         <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,7 +807,7 @@
         <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +829,7 @@
         <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,7 +851,7 @@
         <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -867,7 +873,7 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,7 +895,7 @@
         <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,7 +906,7 @@
         <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -933,7 +939,7 @@
         <v>72</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -977,7 +983,7 @@
         <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -988,7 +994,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>